<commit_message>
updated ts, td, py and remove temp files
</commit_message>
<xml_diff>
--- a/py.projects/testdata.xlsx
+++ b/py.projects/testdata.xlsx
@@ -241,13 +241,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N13" activeCellId="0" sqref="N13"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.9"/>
@@ -350,6 +350,10 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://www.saucedemo.com/"/>

</xml_diff>